<commit_message>
added ability to have custom suffix replacement
</commit_message>
<xml_diff>
--- a/tests/test_data/test_full_ar6.xlsx
+++ b/tests/test_data/test_full_ar6.xlsx
@@ -96,28 +96,28 @@
     <t xml:space="preserve">sspn</t>
   </si>
   <si>
-    <t xml:space="preserve">prefix|Emissions|BC|Harmonized-DB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prefix|Emissions|BC|sector1|Harmonized-DB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prefix|Emissions|BC|setcor2|Harmonized-DB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prefix|Emissions|Sulfur|Harmonized-DB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prefix|Emissions|OC|Harmonized-DB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prefix|Emissions|CH4|Harmonized-DB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prefix|Emissions|CH4|sector1|Harmonized-DB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prefix|Emissions|CH4|sector2|Harmonized-DB</t>
+    <t xml:space="preserve">prefix|Emissions|BC|Harmonized</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prefix|Emissions|BC|sector1|Harmonized</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prefix|Emissions|BC|setcor2|Harmonized</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prefix|Emissions|Sulfur|Harmonized</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prefix|Emissions|OC|Harmonized</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prefix|Emissions|CH4|Harmonized</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prefix|Emissions|CH4|sector1|Harmonized</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prefix|Emissions|CH4|sector2|Harmonized</t>
   </si>
 </sst>
 </file>
@@ -222,12 +222,14 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+      <selection pane="topLeft" activeCell="F7" activeCellId="1" sqref="D2:D17 F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="32.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -596,12 +598,14 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+      <selection pane="topLeft" activeCell="G8" activeCellId="1" sqref="D2:D17 G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="32.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1032,12 +1036,14 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="41.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="41.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>